<commit_message>
Files not found mentioned in log.
</commit_message>
<xml_diff>
--- a/catalogueXlsx/catalogue1v001.xlsx
+++ b/catalogueXlsx/catalogue1v001.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11792" uniqueCount="3772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11793" uniqueCount="3772">
   <si>
     <t xml:space="preserve">A.SIZE
 </t>
@@ -11721,8 +11721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q899"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A606" workbookViewId="0">
+      <selection activeCell="Q633" sqref="Q633"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -45253,6 +45253,9 @@
       </c>
       <c r="P633" t="s">
         <v>7</v>
+      </c>
+      <c r="Q633" t="s">
+        <v>2107</v>
       </c>
     </row>
     <row r="634" spans="1:17">

</xml_diff>